<commit_message>
Update Data Dictionary mit Temperatur
</commit_message>
<xml_diff>
--- a/Data Dictionary, Wetter.xlsx
+++ b/Data Dictionary, Wetter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiman\Documents\Gruppe 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6213D90-7464-47B2-89BB-6BDFD43D181E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF76767-2066-45FC-B5BB-CD6828CEEF40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,20 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Sturm</t>
   </si>
@@ -136,6 +144,39 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>Temperatur</t>
+  </si>
+  <si>
+    <t>Eistag</t>
+  </si>
+  <si>
+    <t>-10 - 0</t>
+  </si>
+  <si>
+    <t>Kalttag</t>
+  </si>
+  <si>
+    <t>Warmtag</t>
+  </si>
+  <si>
+    <t>16-24</t>
+  </si>
+  <si>
+    <t>Sommertag</t>
+  </si>
+  <si>
+    <t>25-30</t>
+  </si>
+  <si>
+    <t>Hitzetag</t>
+  </si>
+  <si>
+    <t>31-40</t>
+  </si>
+  <si>
+    <t>1-15</t>
   </si>
 </sst>
 </file>
@@ -185,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +249,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -548,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,10 +777,10 @@
       <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -781,6 +825,77 @@
         <v>8</v>
       </c>
       <c r="C23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="3">
         <v>4</v>
       </c>
     </row>

</xml_diff>